<commit_message>
Finished code to generate FAST input files w/new dictionary
Still need to verify the calculations though.
</commit_message>
<xml_diff>
--- a/FAST_models/WindPACT/excel_proc/turbines/1.5A08V03_proc.xlsx
+++ b/FAST_models/WindPACT/excel_proc/turbines/1.5A08V03_proc.xlsx
@@ -4498,11 +4498,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="319062096"/>
-        <c:axId val="319061312"/>
+        <c:axId val="307190288"/>
+        <c:axId val="307189896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="319062096"/>
+        <c:axId val="307190288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4587,12 +4587,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319061312"/>
+        <c:crossAx val="307189896"/>
         <c:crossesAt val="-10"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="319061312"/>
+        <c:axId val="307189896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4676,7 +4676,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319062096"/>
+        <c:crossAx val="307190288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11060,7 +11060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>

</xml_diff>